<commit_message>
Update meta data, added new problem
</commit_message>
<xml_diff>
--- a/LeetCode/meta_data.xlsx
+++ b/LeetCode/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\+Machine_Learning_Journey\contributions\Data_Structure_and_Algorithms\DS_and_Algo\main\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8528900E-26ED-4C52-8936-3743DAF29A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1006CBB8-4414-43D4-92C3-535DA9831D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Problem</t>
   </si>
@@ -114,13 +114,25 @@
     <t>Longest Palindromic Substring</t>
   </si>
   <si>
-    <t>longest_sub_palindrom</t>
-  </si>
-  <si>
     <t>Brute-Force, two separate cases (even / odd)</t>
   </si>
   <si>
     <t>look at the size of problem. Somtime, the brute-force might be the only way!</t>
+  </si>
+  <si>
+    <t>zigzag conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move pointer, and change direction if necessary </t>
+  </si>
+  <si>
+    <t>Instead of (I,j) in  a 2D list, sometimes  it is enough to just use one cursor of rows. // Also, try to consider more test cases (e.g. you can randomly generate `s` of different length, and consider `numRows` from 0 to len(s) )</t>
+  </si>
+  <si>
+    <t>longest_sub_palindrom.py</t>
+  </si>
+  <si>
+    <t>zigzag_convertor.py</t>
   </si>
 </sst>
 </file>
@@ -467,18 +479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="7" max="7" width="44" customWidth="1"/>
     <col min="8" max="9" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -600,7 +612,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -608,7 +620,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
@@ -617,21 +629,35 @@
         <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -771,8 +797,9 @@
     <hyperlink ref="E4" r:id="rId3" xr:uid="{0EE61AAE-3359-4CD1-9CC7-DB1CF567A337}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{27568403-A0D7-4FF9-8DC5-4118878E2563}"/>
     <hyperlink ref="E6" r:id="rId5" xr:uid="{4D3D49E8-195C-4898-9F2E-6D5211E9FC88}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{C55159F0-3A1B-49BC-A76B-60AFA1BF6194}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add naive implementation WIP
</commit_message>
<xml_diff>
--- a/LeetCode/meta_data.xlsx
+++ b/LeetCode/meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\+Machine_Learning_Journey\contributions\Data_Structure_and_Algorithms\DS_and_Algo\main\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B741002-AD26-4186-A005-66F801AA5DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A74E15C-96BA-4463-B03D-0593D6A35150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Problem</t>
   </si>
@@ -142,13 +142,28 @@
   </si>
   <si>
     <t>string reverse</t>
+  </si>
+  <si>
+    <t>regular expression match</t>
+  </si>
+  <si>
+    <t>my_re_match.py</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>string parsing</t>
+  </si>
+  <si>
+    <t>TBD! (for now: try to find different cases / scenarios)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,13 +187,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -194,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,6 +231,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -489,7 +520,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,14 +722,28 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -820,8 +865,9 @@
     <hyperlink ref="E6" r:id="rId5" xr:uid="{4D3D49E8-195C-4898-9F2E-6D5211E9FC88}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{C55159F0-3A1B-49BC-A76B-60AFA1BF6194}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{AE90AF8B-31EF-4651-8EF0-1DA01912C7CD}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{CEC3FCB5-3FD9-4D73-9B4D-E31D6188A662}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add a few more functions and update meta
</commit_message>
<xml_diff>
--- a/LeetCode/meta_data.xlsx
+++ b/LeetCode/meta_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\+Machine_Learning_Journey\contributions\Data_Structure_and_Algorithms\DS_and_Algo\main\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CC2DD5-5773-419C-9617-224ACEF68207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC7F9F2-2A9D-4C6F-A83E-6DCD4E4CA283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11628" yWindow="0" windowWidth="11412" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t>Problem</t>
   </si>
@@ -210,10 +210,56 @@
     <t>three_sum.py</t>
   </si>
   <si>
-    <t>fix one, and use two pointers on the rest!</t>
-  </si>
-  <si>
     <t>sorting, and two pointers</t>
+  </si>
+  <si>
+    <t>3SumClosest</t>
+  </si>
+  <si>
+    <t>three_sum_closest.py</t>
+  </si>
+  <si>
+    <t>sorting, two pointers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix one at idx, and then use two pointers at i=idx+1 and j=last index </t>
+  </si>
+  <si>
+    <t>fix one, and use two pointers on the rest! (Also: see `three_sum_closest.py` as it has cleaner / better implementation)</t>
+  </si>
+  <si>
+    <t>letter combination</t>
+  </si>
+  <si>
+    <t>letter_combinations.py</t>
+  </si>
+  <si>
+    <t>dynamic programming</t>
+  </si>
+  <si>
+    <r>
+      <t>use helper function to calculate output dynamically. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>How about recursively? Think</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -579,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,7 +1007,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -978,34 +1024,66 @@
         <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="2" t="s">
         <v>61</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -1064,8 +1142,10 @@
     <hyperlink ref="E14" r:id="rId13" xr:uid="{55DEE963-AE52-4AFE-B544-A5BDD3BB7E1A}"/>
     <hyperlink ref="E15" r:id="rId14" xr:uid="{FAD0FC42-F297-4737-BCDB-59070FFAB440}"/>
     <hyperlink ref="E16" r:id="rId15" xr:uid="{E82CCF2B-63B8-46A7-BE41-9E28C8D1CBEB}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{C66448A5-4730-4A3F-9E7F-B0661BF8FF46}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{3A14DBCD-44F6-4850-A3E1-0F27F1BCF8C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding several new functions
</commit_message>
<xml_diff>
--- a/LeetCode/meta_data.xlsx
+++ b/LeetCode/meta_data.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\+Machine_Learning_Journey\contributions\Data_Structure_and_Algorithms\DS_and_Algo\main\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC7F9F2-2A9D-4C6F-A83E-6DCD4E4CA283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF861E93-4508-42CE-A921-DAC80A9B9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="89">
   <si>
     <t>Problem</t>
   </si>
@@ -260,6 +270,61 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>4Sum</t>
+  </si>
+  <si>
+    <t>Q: Could you do this in one pass? 
+(slow/fast pointers?)</t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>remove_Nth_node_linkedlist.py</t>
+  </si>
+  <si>
+    <t>traverse once, and then traverse again!</t>
+  </si>
+  <si>
+    <t>Valid Paranthesis</t>
+  </si>
+  <si>
+    <t>use stack (and hash)</t>
+  </si>
+  <si>
+    <t>understand that at somepoint after an opening char, you need the same closing char!</t>
+  </si>
+  <si>
+    <t>is_valid_paranthesis.py</t>
+  </si>
+  <si>
+    <t>Merge two sorted linkedlist</t>
+  </si>
+  <si>
+    <t>merge_two_sorted_linkedlist.py</t>
+  </si>
+  <si>
+    <t>traversing both parallel to each other and pick the smaller one</t>
+  </si>
+  <si>
+    <t>linkedlist traversal</t>
+  </si>
+  <si>
+    <t>generate paranthesis</t>
+  </si>
+  <si>
+    <t>generate_paranthesis.py</t>
+  </si>
+  <si>
+    <t>can you do it recursively?</t>
+  </si>
+  <si>
+    <t>Merge k sorted linkedlist</t>
+  </si>
+  <si>
+    <t>merged_k_sorted_linkedlist</t>
   </si>
 </sst>
 </file>
@@ -298,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -341,6 +412,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,21 +703,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="25.109375" customWidth="1"/>
     <col min="4" max="4" width="7.77734375" customWidth="1"/>
     <col min="5" max="5" width="9.44140625" customWidth="1"/>
     <col min="6" max="6" width="18.88671875" customWidth="1"/>
     <col min="7" max="7" width="44" customWidth="1"/>
-    <col min="8" max="9" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1086,44 +1168,294 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1144,8 +1476,14 @@
     <hyperlink ref="E16" r:id="rId15" xr:uid="{E82CCF2B-63B8-46A7-BE41-9E28C8D1CBEB}"/>
     <hyperlink ref="E17" r:id="rId16" xr:uid="{C66448A5-4730-4A3F-9E7F-B0661BF8FF46}"/>
     <hyperlink ref="E18" r:id="rId17" xr:uid="{3A14DBCD-44F6-4850-A3E1-0F27F1BCF8C0}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{3299EFDA-7E1E-4F0E-AC1A-847D934D8491}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{AE801735-7D20-4F44-A95D-D8B315225B98}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{0D843726-ABD3-40FD-856C-FEA7EE663562}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{123D73E6-6AC3-49C2-B282-B953F06FEAAC}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{B6A09A69-EED4-4987-B9D2-D839202498E9}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{4C3720D3-35AE-447A-8984-8559BAE45742}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>